<commit_message>
Working on sustainable consumption rate graph.
</commit_message>
<xml_diff>
--- a/chapters/ch05-ResourceIntensity/datasets/Graedel_Allenby_Sustainable_Resource_Use_Tables.xlsx
+++ b/chapters/ch05-ResourceIntensity/datasets/Graedel_Allenby_Sustainable_Resource_Use_Tables.xlsx
@@ -8,27 +8,37 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/MCBook2021/chapters/ch05-ResourceIntensity/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52B2F388-C647-B94E-B0A1-25324985752E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53AE7828-A04F-9D47-9458-8EDC3CB61F57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11580" yWindow="5460" windowWidth="28040" windowHeight="17440" activeTab="3" xr2:uid="{F1A02A42-1B8A-024E-9938-51155CC88EDB}"/>
+    <workbookView xWindow="760" yWindow="560" windowWidth="28040" windowHeight="17440" xr2:uid="{F1A02A42-1B8A-024E-9938-51155CC88EDB}"/>
   </bookViews>
   <sheets>
-    <sheet name="meta" sheetId="2" r:id="rId1"/>
-    <sheet name="Zinc" sheetId="1" r:id="rId2"/>
-    <sheet name="Germanium" sheetId="3" r:id="rId3"/>
-    <sheet name="CO2" sheetId="5" r:id="rId4"/>
+    <sheet name="data to plot" sheetId="6" r:id="rId1"/>
+    <sheet name="meta" sheetId="2" r:id="rId2"/>
+    <sheet name="Zinc" sheetId="1" r:id="rId3"/>
+    <sheet name="Germanium" sheetId="3" r:id="rId4"/>
+    <sheet name="CO2" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="42">
   <si>
     <t>Global reserve</t>
   </si>
@@ -136,16 +146,41 @@
   </si>
   <si>
     <t>Per capita US emission rate</t>
+  </si>
+  <si>
+    <t>Substance</t>
+  </si>
+  <si>
+    <t>Multiple_of_sustainable</t>
+  </si>
+  <si>
+    <t>Germanium</t>
+  </si>
+  <si>
+    <t>Zinc</t>
+  </si>
+  <si>
+    <t>CO2</t>
+  </si>
+  <si>
+    <t>Resource</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -171,10 +206,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -488,6 +524,57 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A86AA6A-5923-C64E-9B98-E5CAE5139D16}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="str">
+        <f>Zinc!E5</f>
+        <v>Zinc</v>
+      </c>
+      <c r="B2">
+        <f>Zinc!E24</f>
+        <v>5.3667262969588547</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="str">
+        <f>Germanium!E5</f>
+        <v>Germanium</v>
+      </c>
+      <c r="B3">
+        <f>Germanium!E24</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="str">
+        <f>'CO2'!E5</f>
+        <v>CO2</v>
+      </c>
+      <c r="B4">
+        <f>'CO2'!E23</f>
+        <v>6.6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13EAAA9C-5E6C-B047-9190-6FF405FBADB6}">
   <dimension ref="A4:E9"/>
   <sheetViews>
@@ -548,12 +635,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEE1F513-86F8-5D4F-B25A-A1CFC9631808}">
-  <dimension ref="D7:G24"/>
+  <dimension ref="D5:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24:E24"/>
+      <selection activeCell="E5" sqref="D5:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -561,6 +648,14 @@
     <col min="4" max="4" width="21.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="5" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" t="s">
+        <v>39</v>
+      </c>
+    </row>
     <row r="7" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D7" t="s">
         <v>0</v>
@@ -708,12 +803,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4D88768-E398-3743-B04E-70C4E20D6CA6}">
-  <dimension ref="D7:G24"/>
+  <dimension ref="D5:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -721,6 +816,14 @@
     <col min="4" max="4" width="24.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="5" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" t="s">
+        <v>38</v>
+      </c>
+    </row>
     <row r="7" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D7" t="s">
         <v>22</v>
@@ -868,12 +971,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4360E037-F228-104B-9DE7-0BBC774946D7}">
-  <dimension ref="D7:H23"/>
+  <dimension ref="D5:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -881,6 +984,14 @@
     <col min="4" max="4" width="21.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="5" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
     <row r="7" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D7" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
Zinc --> zinc; Germanium --> gemanium
</commit_message>
<xml_diff>
--- a/chapters/ch05-ResourceIntensity/datasets/Graedel_Allenby_Sustainable_Resource_Use_Tables.xlsx
+++ b/chapters/ch05-ResourceIntensity/datasets/Graedel_Allenby_Sustainable_Resource_Use_Tables.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/MCBook2021/chapters/ch05-ResourceIntensity/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53AE7828-A04F-9D47-9458-8EDC3CB61F57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8EC9220-7564-E240-B851-50DD6EAE5EF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="560" windowWidth="28040" windowHeight="17440" xr2:uid="{F1A02A42-1B8A-024E-9938-51155CC88EDB}"/>
   </bookViews>
@@ -154,16 +154,16 @@
     <t>Multiple_of_sustainable</t>
   </si>
   <si>
-    <t>Germanium</t>
-  </si>
-  <si>
-    <t>Zinc</t>
-  </si>
-  <si>
     <t>CO2</t>
   </si>
   <si>
     <t>Resource</t>
+  </si>
+  <si>
+    <t>zinc</t>
+  </si>
+  <si>
+    <t>germanium</t>
   </si>
 </sst>
 </file>
@@ -527,13 +527,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A86AA6A-5923-C64E-9B98-E5CAE5139D16}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B1" t="s">
         <v>37</v>
@@ -542,7 +544,7 @@
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
         <f>Zinc!E5</f>
-        <v>Zinc</v>
+        <v>zinc</v>
       </c>
       <c r="B2">
         <f>Zinc!E24</f>
@@ -552,7 +554,7 @@
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
         <f>Germanium!E5</f>
-        <v>Germanium</v>
+        <v>germanium</v>
       </c>
       <c r="B3">
         <f>Germanium!E24</f>
@@ -640,7 +642,7 @@
   <dimension ref="D5:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="D5:E5"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -653,7 +655,7 @@
         <v>36</v>
       </c>
       <c r="E5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="4:7" x14ac:dyDescent="0.2">
@@ -808,7 +810,7 @@
   <dimension ref="D5:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -821,7 +823,7 @@
         <v>36</v>
       </c>
       <c r="E5" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="4:7" x14ac:dyDescent="0.2">
@@ -989,7 +991,7 @@
         <v>36</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="4:8" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Working on weak/strong sustainability.
</commit_message>
<xml_diff>
--- a/chapters/ch05-ResourceIntensity/datasets/Graedel_Allenby_Sustainable_Resource_Use_Tables.xlsx
+++ b/chapters/ch05-ResourceIntensity/datasets/Graedel_Allenby_Sustainable_Resource_Use_Tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/MCBook2021/chapters/ch05-ResourceIntensity/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8EC9220-7564-E240-B851-50DD6EAE5EF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65A521FD-7187-D645-B76B-C90E16119292}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="560" windowWidth="28040" windowHeight="17440" xr2:uid="{F1A02A42-1B8A-024E-9938-51155CC88EDB}"/>
+    <workbookView xWindow="760" yWindow="760" windowWidth="28040" windowHeight="17440" xr2:uid="{F1A02A42-1B8A-024E-9938-51155CC88EDB}"/>
   </bookViews>
   <sheets>
     <sheet name="data to plot" sheetId="6" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="42">
   <si>
     <t>Global reserve</t>
   </si>
@@ -151,9 +151,6 @@
     <t>Substance</t>
   </si>
   <si>
-    <t>Multiple_of_sustainable</t>
-  </si>
-  <si>
     <t>CO2</t>
   </si>
   <si>
@@ -164,6 +161,9 @@
   </si>
   <si>
     <t>germanium</t>
+  </si>
+  <si>
+    <t>rho</t>
   </si>
 </sst>
 </file>
@@ -528,17 +528,17 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -547,8 +547,8 @@
         <v>zinc</v>
       </c>
       <c r="B2">
-        <f>Zinc!E24</f>
-        <v>5.3667262969588547</v>
+        <f>Zinc!E25 * 100</f>
+        <v>436.67262969588546</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -557,8 +557,8 @@
         <v>germanium</v>
       </c>
       <c r="B3">
-        <f>Germanium!E24</f>
-        <v>2</v>
+        <f>Germanium!E25 * 100</f>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -567,8 +567,8 @@
         <v>CO2</v>
       </c>
       <c r="B4">
-        <f>'CO2'!E23</f>
-        <v>6.6</v>
+        <f>'CO2'!E24 * 100</f>
+        <v>560</v>
       </c>
     </row>
   </sheetData>
@@ -639,10 +639,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEE1F513-86F8-5D4F-B25A-A1CFC9631808}">
-  <dimension ref="D5:G24"/>
+  <dimension ref="D5:G25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -655,7 +655,7 @@
         <v>36</v>
       </c>
       <c r="E5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="4:7" x14ac:dyDescent="0.2">
@@ -797,6 +797,15 @@
       <c r="E24">
         <f>E21/E12</f>
         <v>5.3667262969588547</v>
+      </c>
+    </row>
+    <row r="25" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D25" t="s">
+        <v>41</v>
+      </c>
+      <c r="E25">
+        <f>E24-1</f>
+        <v>4.3667262969588547</v>
       </c>
     </row>
   </sheetData>
@@ -807,10 +816,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4D88768-E398-3743-B04E-70C4E20D6CA6}">
-  <dimension ref="D5:G24"/>
+  <dimension ref="D5:G25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -823,7 +832,7 @@
         <v>36</v>
       </c>
       <c r="E5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="4:7" x14ac:dyDescent="0.2">
@@ -965,6 +974,15 @@
       <c r="E24">
         <f>E21/E12</f>
         <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D25" t="s">
+        <v>41</v>
+      </c>
+      <c r="E25">
+        <f>E24-1</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -975,10 +993,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4360E037-F228-104B-9DE7-0BBC774946D7}">
-  <dimension ref="D5:H23"/>
+  <dimension ref="D5:H24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -991,7 +1009,7 @@
         <v>36</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="4:8" x14ac:dyDescent="0.2">
@@ -1126,6 +1144,15 @@
       <c r="E23" s="2">
         <f>E20/E12</f>
         <v>6.6</v>
+      </c>
+    </row>
+    <row r="24" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D24" t="s">
+        <v>41</v>
+      </c>
+      <c r="E24">
+        <f>E23-1</f>
+        <v>5.6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>